<commit_message>
/ ‘Extended Campuses/Self Appraisals/2016/TME SQL Raw Data from Jan-June 2016.xlsx’
</commit_message>
<xml_diff>
--- a/Extended Campuses/Self Appraisals/2016/TME SQL Raw Data from Jan-June 2016.xlsx
+++ b/Extended Campuses/Self Appraisals/2016/TME SQL Raw Data from Jan-June 2016.xlsx
@@ -917,8 +917,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:G140"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="G110" sqref="G110"/>
+    <sheetView tabSelected="1" topLeftCell="A110" workbookViewId="0">
+      <selection activeCell="G110" sqref="G110:G126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
/ ‘Extended Campuses/Self Appraisals/2016/Self App Summary.docx’ / ‘Extended Campuses/Self Appraisals/2016/TME SQL Raw Data from Jan-June 2016.xlsx’
</commit_message>
<xml_diff>
--- a/Extended Campuses/Self Appraisals/2016/TME SQL Raw Data from Jan-June 2016.xlsx
+++ b/Extended Campuses/Self Appraisals/2016/TME SQL Raw Data from Jan-June 2016.xlsx
@@ -917,8 +917,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:G140"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A125" workbookViewId="0">
-      <selection activeCell="E129" sqref="E129:G133"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41:E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1852,7 +1852,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>240</v>
       </c>
@@ -1875,7 +1875,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>240</v>
       </c>
@@ -1898,7 +1898,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>240</v>
       </c>
@@ -1921,7 +1921,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>240</v>
       </c>
@@ -1944,7 +1944,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>240</v>
       </c>
@@ -1967,7 +1967,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>240</v>
       </c>
@@ -1990,7 +1990,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>240</v>
       </c>
@@ -2013,7 +2013,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>240</v>
       </c>
@@ -2036,7 +2036,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>240</v>
       </c>
@@ -2059,7 +2059,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>240</v>
       </c>
@@ -2082,7 +2082,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>240</v>
       </c>
@@ -2105,7 +2105,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>240</v>
       </c>
@@ -2128,7 +2128,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>240</v>
       </c>
@@ -2151,7 +2151,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>240</v>
       </c>
@@ -2174,7 +2174,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>240</v>
       </c>
@@ -2197,7 +2197,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>240</v>
       </c>
@@ -2220,7 +2220,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>240</v>
       </c>
@@ -2243,7 +2243,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="58" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>240</v>
       </c>
@@ -2266,7 +2266,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>240</v>
       </c>
@@ -2289,7 +2289,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>240</v>
       </c>
@@ -2312,7 +2312,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>240</v>
       </c>
@@ -2335,7 +2335,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>240</v>
       </c>
@@ -2358,7 +2358,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>240</v>
       </c>
@@ -2519,7 +2519,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="70" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>240</v>
       </c>
@@ -2542,7 +2542,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>240</v>
       </c>
@@ -2565,7 +2565,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="72" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>240</v>
       </c>
@@ -2588,7 +2588,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>240</v>
       </c>
@@ -2611,7 +2611,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="74" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>240</v>
       </c>
@@ -2726,7 +2726,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="79" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>240</v>
       </c>
@@ -2749,7 +2749,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="80" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>240</v>
       </c>
@@ -2772,7 +2772,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="81" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>240</v>
       </c>
@@ -2795,7 +2795,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="82" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>240</v>
       </c>
@@ -2818,7 +2818,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="83" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>240</v>
       </c>
@@ -3439,7 +3439,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="110" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>311</v>
       </c>
@@ -3462,7 +3462,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="111" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>311</v>
       </c>
@@ -3485,7 +3485,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="112" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>311</v>
       </c>
@@ -3508,7 +3508,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="113" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>311</v>
       </c>
@@ -3531,7 +3531,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="114" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>311</v>
       </c>
@@ -3554,7 +3554,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="115" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>311</v>
       </c>
@@ -3577,7 +3577,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="116" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>311</v>
       </c>
@@ -3600,7 +3600,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="117" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>311</v>
       </c>
@@ -3623,7 +3623,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="118" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>311</v>
       </c>
@@ -3646,7 +3646,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="119" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>311</v>
       </c>
@@ -3669,7 +3669,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="120" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>311</v>
       </c>
@@ -3692,7 +3692,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="121" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>311</v>
       </c>
@@ -3715,7 +3715,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="122" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>311</v>
       </c>
@@ -3738,7 +3738,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="123" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>311</v>
       </c>
@@ -3761,7 +3761,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="124" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>311</v>
       </c>
@@ -3784,7 +3784,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="125" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>311</v>
       </c>
@@ -3807,7 +3807,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="126" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>311</v>
       </c>
@@ -3830,7 +3830,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="127" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>311</v>
       </c>
@@ -3853,7 +3853,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="128" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>311</v>
       </c>
@@ -3876,7 +3876,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="129" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>311</v>
       </c>
@@ -3899,7 +3899,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="130" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>311</v>
       </c>
@@ -3922,7 +3922,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="131" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>311</v>
       </c>
@@ -3945,7 +3945,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="132" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>311</v>
       </c>
@@ -3968,7 +3968,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="133" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>311</v>
       </c>
@@ -4156,7 +4156,7 @@
   <autoFilter ref="F1:F140">
     <filterColumn colId="0">
       <filters>
-        <filter val="EC, Yuma, Yav, PL Widget Maintenance"/>
+        <filter val="PL Admin Tools"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>